<commit_message>
improved algorithm, tests and added comments
</commit_message>
<xml_diff>
--- a/testSolutions/VerfrühtesAbbiegenaufWald.xlsx
+++ b/testSolutions/VerfrühtesAbbiegenaufWald.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hpe-my.sharepoint.com/personal/melanie_stach_hpe_com/Documents/Documents/02_Theorie/6.Semester/KI/Lösungen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wetzelm\OneDrive - Hewlett Packard Enterprise\DHBW\KI\a-star-algorithm\testSolutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E7D6D5F-A44B-4680-8111-5AD1A9809D01}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11208"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="20850" windowHeight="11210"/>
   </bookViews>
   <sheets>
     <sheet name="VerfrühtesAbbiegenaufWald" sheetId="1" r:id="rId1"/>
@@ -61,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -545,9 +544,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -906,12 +906,12 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>5</v>
       </c>
@@ -958,7 +958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>5</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>5</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1347,7 +1347,7 @@
       <c r="D10">
         <v>5</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>3</v>
       </c>
       <c r="F10" s="1">
@@ -1381,7 +1381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1397,7 +1397,7 @@
       <c r="E11" s="1">
         <v>5</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="2">
         <v>5</v>
       </c>
       <c r="G11">
@@ -1428,7 +1428,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>5</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>4</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>5</v>
       </c>
@@ -1720,6 +1720,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009FBF8661AD2E354FAE87329803412157" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c16c4dd9e2e32f088242a579a7e24e23">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1e44a191-92cd-4afa-9687-f5bf1469df19" xmlns:ns4="6b5e8f27-ce12-4388-9f1e-22f0df822b36" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="25951810f8527d332c4c5b5f678f3a0e" ns3:_="" ns4:_="">
     <xsd:import namespace="1e44a191-92cd-4afa-9687-f5bf1469df19"/>
@@ -1942,22 +1957,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B7A7860-24AB-406E-9A2D-2F086B0D696F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="1e44a191-92cd-4afa-9687-f5bf1469df19"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6b5e8f27-ce12-4388-9f1e-22f0df822b36"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3637E381-8704-4197-AF5A-75176E72E664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09CCDEC3-F5E9-415E-BBDE-0CBC8BEBA333}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1974,29 +1999,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3637E381-8704-4197-AF5A-75176E72E664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B7A7860-24AB-406E-9A2D-2F086B0D696F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="1e44a191-92cd-4afa-9687-f5bf1469df19"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6b5e8f27-ce12-4388-9f1e-22f0df822b36"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>